<commit_message>
refactoring the class into modular function
</commit_message>
<xml_diff>
--- a/Raw_Data/F037_For_PR_DAM.xlsx
+++ b/Raw_Data/F037_For_PR_DAM.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Doc. No</t>
   </si>
@@ -66,17 +66,20 @@
   <si>
     <t>2024-03</t>
   </si>
+  <si>
+    <t>25.08.2022</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;RM&quot;* #,##0.00_-;\-&quot;RM&quot;* #,##0.00_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;RM&quot;* #,##0_-;\-&quot;RM&quot;* #,##0_-;_-&quot;RM&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="dd\-mmm\-yy"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -127,6 +130,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -141,8 +159,108 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,121 +273,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -286,187 +289,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,6 +804,89 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -819,234 +905,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="31" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="29" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="26" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="31" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1070,10 +1073,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1723,7 +1726,7 @@
   <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="B13" sqref="B13:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -1842,7 +1845,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" ht="15.25" spans="1:7">
+    <row r="11" spans="1:7">
       <c r="A11" s="27"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -1872,20 +1875,30 @@
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" spans="1:7">
-      <c r="A13" s="35"/>
+      <c r="A13" s="35" t="s">
+        <v>16</v>
+      </c>
       <c r="B13" s="36">
         <f>F12</f>
         <v>36</v>
       </c>
       <c r="C13" s="37"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1">
+        <v>4</v>
+      </c>
       <c r="E13" s="1"/>
-      <c r="F13" s="33"/>
+      <c r="F13" s="33">
+        <f>B13-D13</f>
+        <v>32</v>
+      </c>
       <c r="G13" s="38"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
+      <c r="B14" s="36">
+        <f>F13</f>
+        <v>32</v>
+      </c>
       <c r="C14" s="37"/>
       <c r="D14" s="30"/>
       <c r="E14" s="31"/>

</xml_diff>